<commit_message>
Modifications Rapport et Backlog
Reformulations du  Rapport mi - parcours, et mise a jour du Backlog
</commit_message>
<xml_diff>
--- a/rapport d'avancement.xlsx
+++ b/rapport d'avancement.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="47">
   <si>
     <t>Jalon</t>
   </si>
@@ -143,9 +143,6 @@
     <t>Retard sur la reconnaissance de QR codes et du plateau</t>
   </si>
   <si>
-    <t>retard, difficultés lecture et affichage des images d'une webcam</t>
-  </si>
-  <si>
     <t>Difficultés à générer un JAR executable</t>
   </si>
   <si>
@@ -153,6 +150,18 @@
   </si>
   <si>
     <t>Envoi du projet en archive et recherche sur la compilation de projets.</t>
+  </si>
+  <si>
+    <t>Superposition de l'image à ajouter sur le code déjà reconnu</t>
+  </si>
+  <si>
+    <t>Terminé</t>
+  </si>
+  <si>
+    <t>Erreur pour la compilation d'un des programmes de test</t>
+  </si>
+  <si>
+    <t>Envoi du projet avec certains tests fonctionnels.</t>
   </si>
 </sst>
 </file>
@@ -326,8 +335,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tableau4" displayName="Tableau4" ref="A1:E4" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11" headerRowCellStyle="Normal 2" dataCellStyle="Normal 2">
-  <autoFilter ref="A1:E4"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tableau4" displayName="Tableau4" ref="A1:E7" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11" headerRowCellStyle="Normal 2" dataCellStyle="Normal 2">
+  <autoFilter ref="A1:E7"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Enoncé" dataDxfId="10" dataCellStyle="Normal 2"/>
     <tableColumn id="2" name="Impact" dataDxfId="9" dataCellStyle="Normal 2"/>
@@ -643,7 +652,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -699,9 +708,11 @@
       <c r="B4" s="5">
         <v>42689</v>
       </c>
-      <c r="C4" s="1"/>
+      <c r="C4" s="7">
+        <v>42381</v>
+      </c>
       <c r="D4" s="10" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -711,10 +722,10 @@
       <c r="B5" s="5">
         <v>42706</v>
       </c>
-      <c r="C5" s="1"/>
-      <c r="D5" s="10" t="s">
-        <v>7</v>
-      </c>
+      <c r="C5" s="7">
+        <v>42395</v>
+      </c>
+      <c r="D5" s="10"/>
     </row>
     <row r="6" spans="1:4" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
@@ -725,7 +736,7 @@
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="6" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -737,7 +748,7 @@
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="6" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -749,7 +760,7 @@
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="6" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -774,10 +785,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="A6" sqref="A6:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -832,7 +843,7 @@
         <v>42694</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="E3" s="10" t="s">
         <v>38</v>
@@ -840,10 +851,10 @@
     </row>
     <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" s="10" t="s">
         <v>41</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>42</v>
       </c>
       <c r="C4" s="11">
         <v>42705</v>
@@ -852,8 +863,39 @@
         <v>19</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>43</v>
-      </c>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" s="11">
+        <v>42706</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="10"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="10"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="10"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -868,7 +910,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -928,7 +970,7 @@
         <v>1</v>
       </c>
       <c r="E3" s="16" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>